<commit_message>
amélioration cv et tabSynthese
</commit_message>
<xml_diff>
--- a/assets/doc/tabSynthese.xlsx
+++ b/assets/doc/tabSynthese.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Portfolio\Portfolio\assets\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298BDEC8-33AF-4E22-8DF4-8A1A01F91ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C495C8-2890-40F4-85BD-692459728ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -143,9 +143,6 @@
     <t>TP gestion clients Java</t>
   </si>
   <si>
-    <t xml:space="preserve">Gestions des données </t>
-  </si>
-  <si>
     <t xml:space="preserve">Création de pages web </t>
   </si>
   <si>
@@ -153,6 +150,27 @@
   </si>
   <si>
     <t>Centre de formation : ORT Montreuil</t>
+  </si>
+  <si>
+    <t>Création de graphes pour l'analyse de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Méthode d'envoi de code d'authentification par mail </t>
+  </si>
+  <si>
+    <t>mise en forme de pages webs</t>
+  </si>
+  <si>
+    <t>Réalisation de tableau d'historique d'SMS</t>
+  </si>
+  <si>
+    <t>Conception et intégration de fenêtres applicatives avec gestion des événements</t>
+  </si>
+  <si>
+    <t>Analyse et résolution d’incidents sur les données comptables</t>
+  </si>
+  <si>
+    <t>Optimisation de l’expérience utilisateur sur application mobile</t>
   </si>
 </sst>
 </file>
@@ -162,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +242,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -624,7 +648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -665,18 +689,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -692,15 +704,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -734,29 +770,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1068,11 +1089,11 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
@@ -1081,84 +1102,84 @@
     <col min="44" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1">
+      <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1">
+      <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="43" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="27"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
+    <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1">
+      <c r="A4" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+    <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1">
+      <c r="A5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1">
+      <c r="A6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1180,25 +1201,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="20" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1">
+      <c r="A7" s="29"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="17" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1237,17 +1258,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
+      <c r="A8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1284,21 +1305,21 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="18"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1335,19 +1356,19 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1384,17 +1405,17 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I11"/>
@@ -1433,19 +1454,19 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I12"/>
@@ -1484,19 +1505,19 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="18"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1533,19 +1554,19 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="22" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I14"/>
@@ -1584,15 +1605,15 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="22"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="18"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1629,15 +1650,15 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="22"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="18"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1674,15 +1695,15 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="22"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="18"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1719,15 +1740,15 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="22"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="18"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1764,17 +1785,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
+      <c r="A19" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="31"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1811,21 +1832,23 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="22" t="s">
+      <c r="C20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I20"/>
@@ -1864,21 +1887,23 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="22" t="s">
+      <c r="C21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I21"/>
@@ -1917,15 +1942,25 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+    <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="22"/>
+      <c r="C22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -1962,15 +1997,23 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="22"/>
+      <c r="C23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2007,15 +2050,15 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="22"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="18"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2052,15 +2095,15 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="22"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="18"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2097,15 +2140,15 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="22"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="18"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2142,17 +2185,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999">
+      <c r="A27" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2189,21 +2232,21 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="22" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I28"/>
@@ -2242,21 +2285,21 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="22" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I29"/>
@@ -2295,15 +2338,25 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="15"/>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2340,15 +2393,25 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
+      <c r="A31" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
+      <c r="C31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2385,15 +2448,15 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="18"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2430,15 +2493,15 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="18"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2475,15 +2538,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="43"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2520,7 +2583,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="13.8">
       <c r="A35" s="5"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -2565,59 +2628,54 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:43" customFormat="1"/>
+    <row r="37" spans="1:43" customFormat="1"/>
+    <row r="38" spans="1:43" customFormat="1"/>
+    <row r="39" spans="1:43" customFormat="1"/>
+    <row r="40" spans="1:43" customFormat="1"/>
+    <row r="41" spans="1:43" customFormat="1"/>
+    <row r="42" spans="1:43" customFormat="1"/>
+    <row r="43" spans="1:43" customFormat="1"/>
+    <row r="44" spans="1:43" customFormat="1"/>
+    <row r="45" spans="1:43" customFormat="1"/>
+    <row r="46" spans="1:43" customFormat="1"/>
+    <row r="47" spans="1:43" customFormat="1"/>
+    <row r="48" spans="1:43" customFormat="1"/>
+    <row r="49" customFormat="1"/>
+    <row r="50" customFormat="1"/>
+    <row r="51" customFormat="1"/>
+    <row r="52" customFormat="1"/>
+    <row r="53" customFormat="1"/>
+    <row r="54" customFormat="1"/>
+    <row r="55" customFormat="1"/>
+    <row r="56" customFormat="1"/>
+    <row r="57" customFormat="1"/>
+    <row r="58" customFormat="1"/>
+    <row r="59" customFormat="1"/>
+    <row r="60" customFormat="1"/>
+    <row r="61" customFormat="1"/>
+    <row r="62" customFormat="1"/>
+    <row r="63" customFormat="1"/>
+    <row r="64" customFormat="1"/>
+    <row r="65" customFormat="1"/>
+    <row r="66" customFormat="1"/>
+    <row r="67" customFormat="1"/>
+    <row r="68" customFormat="1"/>
+    <row r="69" customFormat="1"/>
+    <row r="70" customFormat="1"/>
+    <row r="71" customFormat="1"/>
+    <row r="72" customFormat="1"/>
+    <row r="73" customFormat="1"/>
+    <row r="74" customFormat="1"/>
+    <row r="75" customFormat="1"/>
+    <row r="76" customFormat="1"/>
+    <row r="77" customFormat="1"/>
+    <row r="78" customFormat="1"/>
+    <row r="79" customFormat="1"/>
+    <row r="80" customFormat="1"/>
+    <row r="81" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2625,6 +2683,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>